<commit_message>
Many updates to synapse and neuron objects.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Synapse_Data.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Synapse_Data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Scharzenberger\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Multistate_CPG_Phase_Alignment\Robot_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Multistate_CPG_Phase_Alignment\Robot_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B2BB09-1527-45EA-8CD3-DE217FB7F18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B5ED5-4EFA-409E-AC72-2200935F8278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5528829A-B9F4-4840-8404-477AEC04AA78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -230,19 +228,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -566,7 +564,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,389 +578,389 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="C5" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <f t="shared" ref="A6:A19" si="0">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="C6" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="C7" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="C8" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
         <v>2</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
         <v>2</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="C10" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
         <v>2</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="C11" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
         <v>2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="C12" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
         <v>3</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="C13" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
         <v>3</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
         <v>3</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="C15" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
         <v>3</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="C16" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
         <v>4</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="C17" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
         <v>4</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="C18" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
         <v>4</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="10">
-        <v>-0.04</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
         <v>4</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="10">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Many neuron and synapse updates.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Synapse_Data.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Multistate_CPG_Phase_Alignment/Robot_Data/Synapse_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Multistate_CPG_Phase_Alignment\Robot_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B5ED5-4EFA-409E-AC72-2200935F8278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5DC6C5-10A8-4582-98EA-2C1801B4457E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5528829A-B9F4-4840-8404-477AEC04AA78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5528829A-B9F4-4840-8404-477AEC04AA78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>